<commit_message>
fixed allowed float numbers in 'quantidade' and moved some functions for better organization
</commit_message>
<xml_diff>
--- a/gabarito.xlsx
+++ b/gabarito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almox01.filial\Documents\Executaveis\v6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almox01.filial\Documents\Executaveis\v9.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21424EE-D707-42DD-9183-6A0E29B2C0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E77534-E78F-407B-AF42-F18316367B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="158">
   <si>
     <t>codigo</t>
   </si>
@@ -485,6 +485,18 @@
   </si>
   <si>
     <t>DESENGRIPANTE 300ML/200G</t>
+  </si>
+  <si>
+    <t>COLA SPRAY</t>
+  </si>
+  <si>
+    <t>uso na forracao de containeres de exportacao</t>
+  </si>
+  <si>
+    <t>LAMPADA LED BULBO 15W E-27</t>
+  </si>
+  <si>
+    <t>uso na iluminacao dos setores</t>
   </si>
 </sst>
 </file>
@@ -910,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,7 +2078,7 @@
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4">
-        <f>SUM(C50-D50)</f>
+        <f t="shared" ref="E50:E65" si="4">SUM(C50-D50)</f>
         <v>0</v>
       </c>
       <c r="F50" s="5" t="s">
@@ -2089,7 +2101,7 @@
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4">
-        <f>SUM(C51-D51)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F51" s="5" t="s">
@@ -2112,7 +2124,7 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4">
-        <f>SUM(C52-D52)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F52" s="5" t="s">
@@ -2135,7 +2147,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4">
-        <f>SUM(C53-D53)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F53" s="5" t="s">
@@ -2158,7 +2170,7 @@
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4">
-        <f>SUM(C54-D54)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F54" s="5" t="s">
@@ -2181,7 +2193,7 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4">
-        <f>SUM(C55-D55)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F55" s="5" t="s">
@@ -2204,7 +2216,7 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4">
-        <f>SUM(C56-D56)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F56" s="5" t="s">
@@ -2227,7 +2239,7 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4">
-        <f>SUM(C57-D57)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F57" s="5" t="s">
@@ -2250,7 +2262,7 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4">
-        <f>SUM(C58-D58)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F58" s="5" t="s">
@@ -2273,7 +2285,7 @@
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4">
-        <f>SUM(C59-D59)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F59" s="5" t="s">
@@ -2296,7 +2308,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4">
-        <f>SUM(C60-D60)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F60" s="5" t="s">
@@ -2319,7 +2331,7 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4">
-        <f>SUM(C61-D61)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F61" s="5" t="s">
@@ -2342,7 +2354,7 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4">
-        <f>SUM(C62-D62)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F62" s="5" t="s">
@@ -2365,7 +2377,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4">
-        <f>SUM(C63-D63)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F63" s="5" t="s">
@@ -2388,7 +2400,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4">
-        <f>SUM(C64-D64)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F64" s="5" t="s">
@@ -2411,7 +2423,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4">
-        <f>SUM(C65-D65)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F65" s="5" t="s">
@@ -2434,7 +2446,7 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4">
-        <f t="shared" ref="E66:E97" si="4">SUM(C66-D66)</f>
+        <f t="shared" ref="E66:E97" si="5">SUM(C66-D66)</f>
         <v>0</v>
       </c>
       <c r="F66" s="5" t="s">
@@ -2457,7 +2469,7 @@
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F67" s="5" t="s">
@@ -2480,7 +2492,7 @@
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F68" s="5" t="s">
@@ -2503,7 +2515,7 @@
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F69" s="6" t="s">
@@ -2526,7 +2538,7 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F70" s="6" t="s">
@@ -2549,7 +2561,7 @@
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F71" s="6" t="s">
@@ -2572,7 +2584,7 @@
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F72" s="6" t="s">
@@ -2595,7 +2607,7 @@
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F73" s="6" t="s">
@@ -2618,7 +2630,7 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F74" s="6" t="s">
@@ -2641,7 +2653,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F75" s="6" t="s">
@@ -2664,7 +2676,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F76" s="6" t="s">
@@ -2687,7 +2699,7 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F77" s="6" t="s">
@@ -2710,7 +2722,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F78" s="6" t="s">
@@ -2733,7 +2745,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F79" s="6" t="s">
@@ -2756,7 +2768,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F80" s="6" t="s">
@@ -2779,7 +2791,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F81" s="6" t="s">
@@ -2802,7 +2814,7 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F82" s="6" t="s">
@@ -2825,7 +2837,7 @@
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F83" s="6" t="s">
@@ -2848,7 +2860,7 @@
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F84" s="6" t="s">
@@ -2871,7 +2883,7 @@
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F85" s="6" t="s">
@@ -2894,7 +2906,7 @@
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
       <c r="E86" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F86" s="6" t="s">
@@ -2917,7 +2929,7 @@
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F87" s="6" t="s">
@@ -2940,7 +2952,7 @@
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F88" s="6" t="s">
@@ -2963,7 +2975,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F89" s="6" t="s">
@@ -2986,7 +2998,7 @@
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F90" s="6" t="s">
@@ -3009,7 +3021,7 @@
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F91" s="6" t="s">
@@ -3032,7 +3044,7 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F92" s="6" t="s">
@@ -3055,7 +3067,7 @@
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F93" s="6" t="s">
@@ -3078,7 +3090,7 @@
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F94" s="6" t="s">
@@ -3101,7 +3113,7 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F95" s="6" t="s">
@@ -3124,7 +3136,7 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F96" s="5" t="s">
@@ -3147,7 +3159,7 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F97" s="5" t="s">
@@ -3170,7 +3182,7 @@
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4">
-        <f t="shared" ref="E98:E129" si="5">SUM(C98-D98)</f>
+        <f t="shared" ref="E98:E129" si="6">SUM(C98-D98)</f>
         <v>0</v>
       </c>
       <c r="F98" s="5" t="s">
@@ -3193,7 +3205,7 @@
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F99" s="5" t="s">
@@ -3216,7 +3228,7 @@
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F100" s="5" t="s">
@@ -3239,7 +3251,7 @@
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F101" s="5" t="s">
@@ -3262,7 +3274,7 @@
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F102" s="5" t="s">
@@ -3285,7 +3297,7 @@
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F103" s="5" t="s">
@@ -3308,7 +3320,7 @@
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F104" s="5" t="s">
@@ -3331,7 +3343,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F105" s="6" t="s">
@@ -3354,7 +3366,7 @@
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F106" s="6" t="s">
@@ -3377,7 +3389,7 @@
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F107" s="6" t="s">
@@ -3400,7 +3412,7 @@
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F108" s="5" t="s">
@@ -3423,7 +3435,7 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F109" s="5" t="s">
@@ -3446,7 +3458,7 @@
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F110" s="5" t="s">
@@ -3469,7 +3481,7 @@
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F111" s="5" t="s">
@@ -3492,7 +3504,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F112" s="5" t="s">
@@ -3515,7 +3527,7 @@
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F113" s="5" t="s">
@@ -3538,7 +3550,7 @@
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F114" s="6" t="s">
@@ -3561,7 +3573,7 @@
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F115" s="6" t="s">
@@ -3584,7 +3596,7 @@
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F116" s="6" t="s">
@@ -3607,7 +3619,7 @@
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F117" s="7" t="s">
@@ -3630,7 +3642,7 @@
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F118" s="7" t="s">
@@ -3653,7 +3665,7 @@
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F119" s="7" t="s">
@@ -3676,7 +3688,7 @@
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F120" s="7" t="s">
@@ -3699,7 +3711,7 @@
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F121" s="7" t="s">
@@ -3722,7 +3734,7 @@
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F122" s="7" t="s">
@@ -3745,7 +3757,7 @@
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F123" s="7" t="s">
@@ -3768,7 +3780,7 @@
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F124" s="7" t="s">
@@ -3791,7 +3803,7 @@
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F125" s="7" t="s">
@@ -3814,7 +3826,7 @@
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F126" s="7" t="s">
@@ -3837,7 +3849,7 @@
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F127" s="7" t="s">
@@ -3860,7 +3872,7 @@
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F128" s="7" t="s">
@@ -3883,7 +3895,7 @@
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F129" s="7" t="s">
@@ -3906,7 +3918,7 @@
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4">
-        <f t="shared" ref="E130:E134" si="6">SUM(C130-D130)</f>
+        <f t="shared" ref="E130:E134" si="7">SUM(C130-D130)</f>
         <v>0</v>
       </c>
       <c r="F130" s="7" t="s">
@@ -3929,7 +3941,7 @@
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F131" s="7" t="s">
@@ -3952,7 +3964,7 @@
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F132" s="7" t="s">
@@ -3975,7 +3987,7 @@
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F133" s="7" t="s">
@@ -3998,7 +4010,7 @@
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F134" s="7" t="s">
@@ -4021,7 +4033,7 @@
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4">
-        <f t="shared" ref="E135:E137" si="7">SUM(C135-D135)</f>
+        <f t="shared" ref="E135:E137" si="8">SUM(C135-D135)</f>
         <v>0</v>
       </c>
       <c r="F135" s="7" t="s">
@@ -4044,7 +4056,7 @@
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F136" s="7" t="s">
@@ -4067,7 +4079,7 @@
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F137" s="7" t="s">
@@ -4077,6 +4089,52 @@
         <v>32450</v>
       </c>
       <c r="H137" s="4">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>6500120090</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4">
+        <f t="shared" ref="E138" si="9">SUM(C138-D138)</f>
+        <v>0</v>
+      </c>
+      <c r="F138" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G138" s="4">
+        <v>32510</v>
+      </c>
+      <c r="H138" s="4">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>650016003300</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4">
+        <f t="shared" ref="E139" si="10">SUM(C139-D139)</f>
+        <v>0</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G139" s="4">
+        <v>32450</v>
+      </c>
+      <c r="H139" s="4">
         <v>333</v>
       </c>
     </row>

</xml_diff>